<commit_message>
Create launch and task for VScode. Remove Program.cs
</commit_message>
<xml_diff>
--- a/testWrapper/MsTestWrapper/srcTest/listView.xlsx
+++ b/testWrapper/MsTestWrapper/srcTest/listView.xlsx
@@ -12,36 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2r3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3we</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3wer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34wr</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3r</t>
   </si>
 </sst>
 </file>
@@ -92,37 +71,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="11">
+      <c r="K11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="12">
+      <c r="K12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="K13" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Problems with git sync
</commit_message>
<xml_diff>
--- a/testWrapper/MsTestWrapper/srcTest/listView.xlsx
+++ b/testWrapper/MsTestWrapper/srcTest/listView.xlsx
@@ -12,36 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2r3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3we</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3wer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34wr</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3r</t>
   </si>
 </sst>
 </file>
@@ -92,37 +71,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="11">
+      <c r="K11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="12">
+      <c r="K12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="K13" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>